<commit_message>
클라이언트 PM문서 ver2.5 update
</commit_message>
<xml_diff>
--- a/PM문서.xlsx
+++ b/PM문서.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\2021\AirHockey\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1743FD57-C072-49D0-A639-71CB6C6ECE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Polaris Office Sheet" lastEdited="7" lowestEdited="7" rupBuild="9.103.97.45139"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="일정표" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors/>
+  <commentList/>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>2021학년도 2학기 네트워크 게임 프로그래밍 PM 문서</t>
   </si>
@@ -122,210 +124,274 @@
   </si>
   <si>
     <t>21.11.21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>21.11.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>recvCommand 함수 기능을 getClient 스레드 함수 내부로 이전(동일 기능 처리 효율 고려)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>공의 위치만 계산하는 newPosition 함수를 가속도까지 계산하는 updateBall 함수로 변경(동일 기능 처리 효율 고려)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>BALLSIZE 30으로 정의</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>21.11.22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>circuitCollide 함수에 int 형 collideType 인자 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>X,Y_SIDE_COLLIDE 변수 각각 11, 22로 정의(변경 가능)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>checkMoveBall 함수 오류 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>updateBall()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>circuitCollide()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>21.11.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>헤더에 맞춘 데이터별 구조체 별도 추가, 해당 구조체를 넘기는 방식으로 통신 방식 변경 (통신 효율 고려)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>21.11.26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>단일 클라이언트와 통신하는 방식 테스트(check-net 브랜치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>서버와 통신하는 방식 테스트(check-net 브랜치)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>일부 자료형, 통신 방식 클라이언트와 통일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>데이터 상시 송신 오류 해결(데이터 사이즈 통일)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>데이터 리포트 확인을 위해 allocconsole 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>일부 자료형, 통신 방식 서버와 통일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>recv함수와 send함수 스레드로 분리, 스레드로 분리하면서 서버에 connect하는 방식 소폭 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>스레드 함수 구조 서버와 통일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>데이터 상시 송,수신 구현 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>브랜치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>check-net</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>*서버 작업자 임의 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>데이터 상시 송신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>데이터 상시 수신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>21.11.29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>서버 - 클라 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>서버 상시 업데이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>리모트 상시 통신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21.12.07</t>
+  </si>
+  <si>
+    <t>게임에 점수 이미지 추가 및 테이블 이미지 변경</t>
+  </si>
+  <si>
+    <t>21.11.23</t>
+  </si>
+  <si>
+    <t>네트워크 관련 send, recv함수 수정 커맨드를 바꿔가면서 동작하도록 변경</t>
+  </si>
+  <si>
+    <t>게임 리소스 수정</t>
+  </si>
+  <si>
+    <t>게임 클라이언트 수정</t>
+  </si>
+  <si>
+    <t>21.12.2</t>
+  </si>
+  <si>
+    <t>멀티 플레이시에 플레이어들의 위치반전으로 같은 환경에서 게임화면이 이루어지도록 함수 적용</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="22">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="8.0"/>
+      <name val="맑은 고딕"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
       <color theme="11"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11.0"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <color theme="5" tint="-0.249980"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <sz val="11.0"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="맑은 고딕"/>
+      <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599960"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -335,14 +401,199 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -357,7 +608,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -370,7 +620,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -381,7 +630,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -394,7 +642,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -405,7 +652,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -414,7 +660,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -425,7 +670,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -434,7 +678,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -443,7 +686,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -454,7 +696,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -463,7 +704,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -474,54 +714,278 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
@@ -578,73 +1042,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="49">
+    <cellStyle name="20% - 강조색1" xfId="25" builtinId="30"/>
+    <cellStyle name="20% - 강조색2" xfId="29" builtinId="34"/>
+    <cellStyle name="20% - 강조색3" xfId="33" builtinId="38"/>
+    <cellStyle name="20% - 강조색4" xfId="37" builtinId="42"/>
+    <cellStyle name="20% - 강조색5" xfId="41" builtinId="46"/>
+    <cellStyle name="20% - 강조색6" xfId="45" builtinId="50"/>
+    <cellStyle name="40% - 강조색1" xfId="26" builtinId="31"/>
+    <cellStyle name="40% - 강조색2" xfId="30" builtinId="35"/>
+    <cellStyle name="40% - 강조색3" xfId="34" builtinId="39"/>
+    <cellStyle name="40% - 강조색4" xfId="38" builtinId="43"/>
+    <cellStyle name="40% - 강조색5" xfId="42" builtinId="47"/>
+    <cellStyle name="40% - 강조색6" xfId="46" builtinId="51"/>
+    <cellStyle name="60% - 강조색1" xfId="27" builtinId="32"/>
+    <cellStyle name="60% - 강조색2" xfId="31" builtinId="36"/>
+    <cellStyle name="60% - 강조색3" xfId="35" builtinId="40"/>
+    <cellStyle name="60% - 강조색4" xfId="39" builtinId="44"/>
+    <cellStyle name="60% - 강조색5" xfId="43" builtinId="48"/>
+    <cellStyle name="60% - 강조색6" xfId="47" builtinId="52"/>
+    <cellStyle name="강조색1" xfId="24" builtinId="29"/>
+    <cellStyle name="강조색2" xfId="28" builtinId="33"/>
+    <cellStyle name="강조색3" xfId="32" builtinId="37"/>
+    <cellStyle name="강조색4" xfId="36" builtinId="41"/>
+    <cellStyle name="강조색5" xfId="40" builtinId="45"/>
+    <cellStyle name="강조색6" xfId="44" builtinId="49"/>
+    <cellStyle name="경고문" xfId="9" builtinId="11"/>
+    <cellStyle name="계산" xfId="17" builtinId="22"/>
+    <cellStyle name="나쁨" xfId="22" builtinId="27"/>
+    <cellStyle name="메모" xfId="8" builtinId="10"/>
+    <cellStyle name="백분율" xfId="5" builtinId="5"/>
+    <cellStyle name="보통" xfId="23" builtinId="28"/>
+    <cellStyle name="설명텍스트" xfId="48" builtinId="53"/>
+    <cellStyle name="셀 확인" xfId="18" builtinId="23"/>
+    <cellStyle name="쉼표" xfId="3" builtinId="3"/>
+    <cellStyle name="쉼표[0]" xfId="6" builtinId="6"/>
+    <cellStyle name="연결된 셀" xfId="19" builtinId="24"/>
     <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="요약" xfId="20" builtinId="25"/>
+    <cellStyle name="입력" xfId="15" builtinId="20"/>
+    <cellStyle name="제목" xfId="10" builtinId="15"/>
+    <cellStyle name="제목 1" xfId="11" builtinId="16"/>
+    <cellStyle name="제목 2" xfId="12" builtinId="17"/>
+    <cellStyle name="제목 3" xfId="13" builtinId="18"/>
+    <cellStyle name="제목 4" xfId="14" builtinId="19"/>
+    <cellStyle name="좋음" xfId="21" builtinId="26"/>
+    <cellStyle name="출력" xfId="16" builtinId="21"/>
+    <cellStyle name="통화" xfId="4" builtinId="4"/>
+    <cellStyle name="통화[0]" xfId="7" builtinId="7"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -944,27 +1417,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AE62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="R52" sqref="R52"/>
+    <sheetView topLeftCell="A52" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S55" sqref="S55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.500000"/>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:31">
+      <c r="B2" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="2:31">
+      <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="24"/>
-    </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:31" ht="17.250000">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1040,13 +1512,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:31">
       <c r="B6" s="5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="16" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1060,34 +1532,34 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
       <c r="AE6" s="7"/>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:31">
       <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="11"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1112,7 +1584,7 @@
       <c r="AD7" s="8"/>
       <c r="AE7" s="10"/>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:31">
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1148,7 +1620,7 @@
       <c r="AD8" s="8"/>
       <c r="AE8" s="10"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:31">
       <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
@@ -1160,10 +1632,10 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -1184,7 +1656,7 @@
       <c r="AD9" s="8"/>
       <c r="AE9" s="10"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:31">
       <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
@@ -1220,11 +1692,11 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="10"/>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:31">
+      <c r="B11" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="11"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1256,8 +1728,8 @@
       <c r="AD11" s="8"/>
       <c r="AE11" s="10"/>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="2:31">
+      <c r="B12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="10"/>
@@ -1292,8 +1764,8 @@
       <c r="AD12" s="8"/>
       <c r="AE12" s="10"/>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+    <row r="13" spans="2:31">
+      <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="10"/>
@@ -1312,10 +1784,10 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
-      <c r="S13" s="23" t="s">
+      <c r="S13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="T13" s="23" t="s">
+      <c r="T13" s="9" t="s">
         <v>4</v>
       </c>
       <c r="U13" s="8"/>
@@ -1330,8 +1802,8 @@
       <c r="AD13" s="8"/>
       <c r="AE13" s="10"/>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+    <row r="14" spans="2:31">
+      <c r="B14" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="10"/>
@@ -1351,10 +1823,10 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="23" t="s">
+      <c r="T14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="U14" s="23" t="s">
+      <c r="U14" s="9" t="s">
         <v>4</v>
       </c>
       <c r="V14" s="8"/>
@@ -1368,8 +1840,8 @@
       <c r="AD14" s="8"/>
       <c r="AE14" s="10"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
+    <row r="15" spans="2:31">
+      <c r="B15" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="10"/>
@@ -1391,10 +1863,10 @@
       <c r="S15" s="8"/>
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
-      <c r="V15" s="23" t="s">
+      <c r="V15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W15" s="23" t="s">
+      <c r="W15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="X15" s="15"/>
@@ -1406,8 +1878,8 @@
       <c r="AD15" s="8"/>
       <c r="AE15" s="10"/>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
+    <row r="16" spans="2:31">
+      <c r="B16" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="10"/>
@@ -1431,7 +1903,7 @@
       <c r="U16" s="15"/>
       <c r="V16" s="15"/>
       <c r="W16" s="15"/>
-      <c r="X16" s="26" t="s">
+      <c r="X16" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Y16" s="15"/>
@@ -1442,8 +1914,8 @@
       <c r="AD16" s="8"/>
       <c r="AE16" s="10"/>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+    <row r="17" spans="2:31">
+      <c r="B17" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="10"/>
@@ -1469,7 +1941,7 @@
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
-      <c r="Z17" s="33" t="s">
+      <c r="Z17" s="9" t="s">
         <v>4</v>
       </c>
       <c r="AA17" s="8"/>
@@ -1478,8 +1950,8 @@
       <c r="AD17" s="8"/>
       <c r="AE17" s="10"/>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B18" s="25"/>
+    <row r="18" spans="2:31">
+      <c r="B18" s="11"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="8"/>
@@ -1510,7 +1982,7 @@
       <c r="AD18" s="8"/>
       <c r="AE18" s="10"/>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:31" ht="17.250000">
       <c r="B19" s="12"/>
       <c r="C19" s="14"/>
       <c r="D19" s="12"/>
@@ -1520,8 +1992,8 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -1542,228 +2014,222 @@
       <c r="AD19" s="13"/>
       <c r="AE19" s="14"/>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="2:31">
+      <c r="B22" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="23" spans="2:31">
+      <c r="B23" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="0" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="2:31">
+      <c r="B24" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="0">
+        <v>1.1</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="25" spans="2:31">
+      <c r="B25" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="0">
         <v>1.2</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
+    <row r="26" spans="2:31">
+      <c r="B26" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="0">
         <v>1.3</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B27" s="24" t="s">
+    <row r="27" spans="2:31">
+      <c r="B27" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="0">
         <v>1.4</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
+    <row r="28" spans="2:31">
+      <c r="B28" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="0">
         <v>1.4</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B29" s="24" t="s">
+    <row r="29" spans="2:31">
+      <c r="B29" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="0">
         <v>1.5</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B30" s="24" t="s">
+    <row r="30" spans="2:31">
+      <c r="B30" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="0">
         <v>1.5</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+    <row r="31" spans="2:31">
+      <c r="B31" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="0">
         <v>1.5</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
+    <row r="32" spans="2:31">
+      <c r="B32" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B33" s="24" t="s">
+    <row r="33" spans="2:31">
+      <c r="B33" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="0">
         <v>2.1</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
+    <row r="34" spans="2:31">
+      <c r="B34" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E34">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F34" s="24" t="s">
+      <c r="E34" s="0">
+        <v>2.2</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="s">
+    <row r="35" spans="2:31">
+      <c r="B35" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E35">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F35" s="24" t="s">
+      <c r="E35" s="0">
+        <v>2.3</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B36" s="24" t="s">
+    <row r="36" spans="2:31">
+      <c r="B36" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="0">
         <v>2.4</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="0" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="41" spans="2:31">
+      <c r="B41" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:31" ht="17.250000">
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
@@ -1803,7 +2269,9 @@
       <c r="P42" s="4">
         <v>22</v>
       </c>
-      <c r="Q42" s="2"/>
+      <c r="Q42" s="2">
+        <v>23</v>
+      </c>
       <c r="R42" s="2">
         <v>2</v>
       </c>
@@ -1820,7 +2288,9 @@
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
+      <c r="Z42" s="2">
+        <v>2</v>
+      </c>
       <c r="AA42" s="2"/>
       <c r="AB42" s="3">
         <v>4</v>
@@ -1835,13 +2305,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:31">
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="16" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
@@ -1855,34 +2325,34 @@
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="32"/>
-      <c r="S43" s="32"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
-      <c r="X43" s="32"/>
-      <c r="Y43" s="32"/>
-      <c r="Z43" s="32"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="6"/>
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
       <c r="AE43" s="7"/>
     </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:31">
       <c r="B44" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="20"/>
       <c r="E44" s="21"/>
-      <c r="F44" s="38" t="s">
+      <c r="F44" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
       <c r="I44" s="21"/>
       <c r="J44" s="16" t="s">
         <v>11</v>
@@ -1909,7 +2379,7 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="10"/>
     </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:31">
       <c r="B45" s="11" t="s">
         <v>23</v>
       </c>
@@ -1945,7 +2415,7 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="10"/>
     </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:31">
       <c r="B46" s="11" t="s">
         <v>24</v>
       </c>
@@ -1981,7 +2451,7 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="10"/>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:31">
       <c r="B47" s="11" t="s">
         <v>25</v>
       </c>
@@ -2017,7 +2487,7 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="10"/>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:31">
       <c r="B48" s="11" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2507,9 @@
       </c>
       <c r="O48" s="8"/>
       <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
+      <c r="Q48" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
@@ -2053,8 +2525,8 @@
       <c r="AD48" s="8"/>
       <c r="AE48" s="10"/>
     </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B49" s="25" t="s">
+    <row r="49" spans="2:31">
+      <c r="B49" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C49" s="10"/>
@@ -2072,7 +2544,7 @@
       <c r="O49" s="8"/>
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
-      <c r="R49" s="33" t="s">
+      <c r="R49" s="9" t="s">
         <v>4</v>
       </c>
       <c r="S49" s="8"/>
@@ -2089,8 +2561,10 @@
       <c r="AD49" s="8"/>
       <c r="AE49" s="10"/>
     </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B50" s="12"/>
+    <row r="50" spans="2:31" ht="17.250000">
+      <c r="B50" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="C50" s="14"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
@@ -2099,8 +2573,8 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
       <c r="O50" s="13"/>
@@ -2114,162 +2588,219 @@
       <c r="W50" s="13"/>
       <c r="X50" s="13"/>
       <c r="Y50" s="13"/>
-      <c r="Z50" s="13"/>
+      <c r="Z50" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="AA50" s="13"/>
       <c r="AB50" s="13"/>
-      <c r="AC50" s="13"/>
-      <c r="AD50" s="13"/>
-      <c r="AE50" s="14"/>
-    </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+      <c r="AC50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE50" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:31">
+      <c r="B53" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D53" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G53" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H53" s="30"/>
-    </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+      <c r="H53" s="25"/>
+    </row>
+    <row r="54" spans="2:31">
+      <c r="B54" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="27" t="s">
+      <c r="E54" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+    <row r="55" spans="2:31">
+      <c r="B55" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D55" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E55">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E55" s="0">
+        <v>1.1</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="24" t="s">
+    <row r="56" spans="2:31">
+      <c r="B56" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="0">
         <v>1.2</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B57" s="28" t="s">
+    <row r="57" spans="2:31">
+      <c r="B57" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E57" s="0">
+        <v>1.3</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="2:31">
+      <c r="B58" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28" t="s">
+      <c r="C58" s="23"/>
+      <c r="D58" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="29" t="s">
+      <c r="E58" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="28" t="s">
+      <c r="F58" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B58" s="28" t="s">
+    <row r="59" spans="2:31">
+      <c r="B59" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28" t="s">
+      <c r="C59" s="23"/>
+      <c r="D59" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="28">
+      <c r="E59" s="23">
         <v>2.1</v>
       </c>
-      <c r="F58" s="28" t="s">
+      <c r="F59" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B59" s="28" t="s">
+    <row r="60" spans="2:31">
+      <c r="B60" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28" t="s">
+      <c r="C60" s="23"/>
+      <c r="D60" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="28">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F59" s="28" t="s">
+      <c r="E60" s="23">
+        <v>2.2</v>
+      </c>
+      <c r="F60" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B60" s="28" t="s">
+    <row r="61" spans="2:31">
+      <c r="B61" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28" t="s">
+      <c r="C61" s="23"/>
+      <c r="D61" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="28">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F60" s="28" t="s">
+      <c r="E61" s="23">
+        <v>2.3</v>
+      </c>
+      <c r="F61" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B61" s="28" t="s">
+    <row r="62" spans="2:31">
+      <c r="B62" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28" t="s">
+      <c r="C62" s="23"/>
+      <c r="D62" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E61" s="28">
+      <c r="E62" s="23">
         <v>2.4</v>
       </c>
-      <c r="F61" s="28" t="s">
+      <c r="F62" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="B62" s="24"/>
+    <row r="63" spans="2:31">
+      <c r="B63" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="0"/>
+      <c r="D63" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="2:31">
+      <c r="B64" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="0"/>
+      <c r="D64" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+      <c r="D65" s="0"/>
+      <c r="E65" s="0"/>
+      <c r="F65" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="K9:L9"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="F44:H44"/>
+    <mergeCell ref="K50:L50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>